<commit_message>
Convert from arrow batch to serialisation
</commit_message>
<xml_diff>
--- a/src/Assets.xlsx
+++ b/src/Assets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kobus\.julia\dev\SAPRINCore\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\SAPRIN_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38A5C29-4882-4249-A39D-DEE3ED13EE0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840D9289-B034-4A6C-B8BF-43438AECDD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12540" yWindow="1890" windowWidth="28800" windowHeight="15460" activeTab="3" xr2:uid="{D2C512BA-B2FB-46F3-9C9F-6F0ED1CF0AB0}"/>
+    <workbookView xWindow="-17388" yWindow="-2412" windowWidth="17496" windowHeight="30216" activeTab="3" xr2:uid="{D2C512BA-B2FB-46F3-9C9F-6F0ED1CF0AB0}"/>
   </bookViews>
   <sheets>
     <sheet name="DIMAMO" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="60">
   <si>
     <t>Stove</t>
   </si>
@@ -191,6 +191,36 @@
   </si>
   <si>
     <t>AssetIdx</t>
+  </si>
+  <si>
+    <t>Lorry/Tractor</t>
+  </si>
+  <si>
+    <t>Swimming pool</t>
+  </si>
+  <si>
+    <t>Air conditioner</t>
+  </si>
+  <si>
+    <t>Computer/Desktop/Laptop</t>
+  </si>
+  <si>
+    <t>Vacuum cleaner/Floor polisher</t>
+  </si>
+  <si>
+    <t>Dish washing machine</t>
+  </si>
+  <si>
+    <t>Tumble dryer</t>
+  </si>
+  <si>
+    <t>Home security service</t>
+  </si>
+  <si>
+    <t>Geyser (providing hot water)</t>
+  </si>
+  <si>
+    <t>Pigs</t>
   </si>
 </sst>
 </file>
@@ -243,6 +273,25 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{430EA748-896E-49FD-AABB-C94C0FD0443F}" name="Table1" displayName="Table1" ref="A1:E47" totalsRowShown="0">
+  <autoFilter ref="A1:E47" xr:uid="{430EA748-896E-49FD-AABB-C94C0FD0443F}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E47">
+    <sortCondition ref="B1:B47"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{A70EA9DE-6BB8-40D7-9F21-E58BF6088A5A}" name="AssetName"/>
+    <tableColumn id="2" xr3:uid="{EAEA389A-AAF8-4F7A-9157-85068A9408B2}" name="AssetId"/>
+    <tableColumn id="3" xr3:uid="{6628AF45-758C-4E98-A76D-8485D7225F23}" name="Name"/>
+    <tableColumn id="4" xr3:uid="{7622E47A-5DE3-483E-804E-8CD3F0D79EAB}" name="Id"/>
+    <tableColumn id="5" xr3:uid="{0E1F3D11-AE5B-4301-A7EB-72A24753FC86}" name="AssetIdx">
+      <calculatedColumnFormula>VLOOKUP(D2,AssetIdx,3,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1588,16 +1637,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F62E7F9A-9D16-4DF2-9A9A-BB3D068650E2}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="A39" sqref="A39:E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
     <col min="3" max="3" width="12.8984375" customWidth="1"/>
+    <col min="5" max="5" width="10.3984375" customWidth="1"/>
+    <col min="7" max="7" width="32.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1925,28 +1977,27 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="B19">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D19">
-        <v>19</v>
-      </c>
-      <c r="E19">
-        <f>VLOOKUP(D19,AssetIdx,3,FALSE)</f>
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
         <v>41</v>
@@ -1961,10 +2012,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
         <v>41</v>
@@ -1979,10 +2030,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
         <v>41</v>
@@ -1997,46 +2048,46 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B23">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23">
-        <v>12</v>
-      </c>
-      <c r="E23" t="str">
+        <v>19</v>
+      </c>
+      <c r="E23">
         <f>VLOOKUP(D23,AssetIdx,3,FALSE)</f>
-        <v>Modern</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B24">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D24">
-        <v>24</v>
-      </c>
-      <c r="E24">
+        <v>12</v>
+      </c>
+      <c r="E24" t="str">
         <f>VLOOKUP(D24,AssetIdx,3,FALSE)</f>
-        <v>0</v>
+        <v>Modern</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
         <v>43</v>
@@ -2051,16 +2102,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D26">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E26">
         <f>VLOOKUP(D26,AssetIdx,3,FALSE)</f>
@@ -2069,34 +2120,34 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="B27">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="D27">
-        <v>27</v>
-      </c>
-      <c r="E27" t="str">
+        <v>19</v>
+      </c>
+      <c r="E27">
         <f>VLOOKUP(D27,AssetIdx,3,FALSE)</f>
-        <v>Livestock</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D28">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E28" t="str">
         <f>VLOOKUP(D28,AssetIdx,3,FALSE)</f>
@@ -2105,70 +2156,70 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B29">
-        <v>100</v>
+        <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D29">
-        <v>100</v>
+        <v>28</v>
       </c>
       <c r="E29" t="str">
         <f>VLOOKUP(D29,AssetIdx,3,FALSE)</f>
-        <v>Modern</v>
+        <v>Livestock</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C30" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D30">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="E30" t="str">
         <f>VLOOKUP(D30,AssetIdx,3,FALSE)</f>
-        <v>Livestock</v>
+        <v>Modern</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B31">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C31" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D31">
-        <v>102</v>
+        <v>28</v>
       </c>
       <c r="E31" t="str">
         <f>VLOOKUP(D31,AssetIdx,3,FALSE)</f>
-        <v>Modern</v>
+        <v>Livestock</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B32">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C32" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D32">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="E32" t="str">
         <f>VLOOKUP(D32,AssetIdx,3,FALSE)</f>
@@ -2177,64 +2228,64 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B33">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="D33">
-        <v>104</v>
-      </c>
-      <c r="E33">
+        <v>12</v>
+      </c>
+      <c r="E33" t="str">
         <f>VLOOKUP(D33,AssetIdx,3,FALSE)</f>
-        <v>0</v>
+        <v>Modern</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B34">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C34" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D34">
-        <v>28</v>
-      </c>
-      <c r="E34" t="str">
+        <v>104</v>
+      </c>
+      <c r="E34">
         <f>VLOOKUP(D34,AssetIdx,3,FALSE)</f>
-        <v>Livestock</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B35">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C35" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="D35">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="E35" t="str">
         <f>VLOOKUP(D35,AssetIdx,3,FALSE)</f>
-        <v>Modern</v>
+        <v>Livestock</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B36">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C36" t="s">
         <v>42</v>
@@ -2249,28 +2300,209 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B37">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C37" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="D37">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E37" t="str">
         <f>VLOOKUP(D37,AssetIdx,3,FALSE)</f>
+        <v>Modern</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38">
+        <v>108</v>
+      </c>
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38">
+        <v>28</v>
+      </c>
+      <c r="E38" t="str">
+        <f>VLOOKUP(D38,AssetIdx,3,FALSE)</f>
         <v>Livestock</v>
       </c>
     </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39">
+        <v>109</v>
+      </c>
+      <c r="C39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39">
+        <v>109</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40">
+        <v>110</v>
+      </c>
+      <c r="C40" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40">
+        <v>12</v>
+      </c>
+      <c r="E40" t="str">
+        <f>VLOOKUP(D40,AssetIdx,3,FALSE)</f>
+        <v>Modern</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41">
+        <v>111</v>
+      </c>
+      <c r="C41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41">
+        <v>12</v>
+      </c>
+      <c r="E41" t="str">
+        <f>VLOOKUP(D41,AssetIdx,3,FALSE)</f>
+        <v>Modern</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42">
+        <v>112</v>
+      </c>
+      <c r="C42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42">
+        <v>12</v>
+      </c>
+      <c r="E42" t="str">
+        <f>VLOOKUP(D42,AssetIdx,3,FALSE)</f>
+        <v>Modern</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43">
+        <v>113</v>
+      </c>
+      <c r="C43" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43">
+        <v>12</v>
+      </c>
+      <c r="E43" t="str">
+        <f>VLOOKUP(D43,AssetIdx,3,FALSE)</f>
+        <v>Modern</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44">
+        <v>114</v>
+      </c>
+      <c r="C44" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44">
+        <v>12</v>
+      </c>
+      <c r="E44" t="str">
+        <f>VLOOKUP(D44,AssetIdx,3,FALSE)</f>
+        <v>Modern</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45">
+        <v>115</v>
+      </c>
+      <c r="C45" t="s">
+        <v>57</v>
+      </c>
+      <c r="D45">
+        <v>115</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46">
+        <v>116</v>
+      </c>
+      <c r="C46" t="s">
+        <v>42</v>
+      </c>
+      <c r="D46">
+        <v>12</v>
+      </c>
+      <c r="E46" t="str">
+        <f>VLOOKUP(D46,AssetIdx,3,FALSE)</f>
+        <v>Modern</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47">
+        <v>120</v>
+      </c>
+      <c r="C47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47">
+        <v>28</v>
+      </c>
+      <c r="E47" t="str">
+        <f>VLOOKUP(D47,AssetIdx,3,FALSE)</f>
+        <v>Livestock</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E37">
-    <sortCondition ref="B2:B37"/>
-    <sortCondition ref="D2:D37"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E38">
+    <sortCondition ref="B2:B38"/>
+    <sortCondition ref="D2:D38"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>